<commit_message>
added competetive_points and work_points
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d7b223cc91b15b5/Projects/ПМЖ/2024-2025^J 7М/8M_Spec_Mat_Analyze/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanu\OneDrive\Projects\ПМЖ\2024-2025, 7М\8M_Spec_Mat_Analyze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6549450-5FC4-4B26-9E5E-893455589F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3738F82B-068A-4622-9D09-99B6757C1558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="problems" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="23">
   <si>
     <t>Тема</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Алгоритм Евклида</t>
+  </si>
+  <si>
+    <t>Сравнение по модулю</t>
   </si>
 </sst>
 </file>
@@ -433,18 +436,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P155"/>
+  <dimension ref="A1:P185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="G160" sqref="G160"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="Q156" sqref="Q156:T185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="16" width="12.7109375" customWidth="1"/>
+    <col min="5" max="16" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -544,7 +547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -594,7 +597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -644,7 +647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -694,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -744,7 +747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -794,7 +797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -844,7 +847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -894,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -944,7 +947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -994,7 +997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1444,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1644,7 +1647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1694,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1744,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1794,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1944,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1994,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2044,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -2244,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -2344,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -2394,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -2494,7 +2497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -2544,7 +2547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -2594,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -2644,7 +2647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -2694,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -2744,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -2844,7 +2847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -2944,7 +2947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -2994,7 +2997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -3044,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -3094,7 +3097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -3144,7 +3147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -3194,7 +3197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -3394,7 +3397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -3444,7 +3447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -3494,7 +3497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -3544,7 +3547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -3594,7 +3597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -3644,7 +3647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -3694,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -3744,7 +3747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -3794,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -3844,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -3894,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -3944,7 +3947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -3994,7 +3997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -4044,7 +4047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -4094,7 +4097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -4144,7 +4147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -4194,7 +4197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>18</v>
       </c>
@@ -4244,7 +4247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -4294,7 +4297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>18</v>
       </c>
@@ -4344,7 +4347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -4394,7 +4397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -4444,7 +4447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>18</v>
       </c>
@@ -4494,7 +4497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -4544,7 +4547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -4594,7 +4597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>18</v>
       </c>
@@ -4644,7 +4647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>18</v>
       </c>
@@ -4694,7 +4697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>18</v>
       </c>
@@ -4744,7 +4747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>18</v>
       </c>
@@ -4794,7 +4797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -4844,7 +4847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -4894,7 +4897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -4944,7 +4947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -4994,7 +4997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -5044,7 +5047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -5094,7 +5097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>18</v>
       </c>
@@ -5144,7 +5147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>18</v>
       </c>
@@ -5194,7 +5197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -5244,7 +5247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>18</v>
       </c>
@@ -5294,7 +5297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>18</v>
       </c>
@@ -5344,7 +5347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>18</v>
       </c>
@@ -5394,7 +5397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>18</v>
       </c>
@@ -5444,7 +5447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>18</v>
       </c>
@@ -5494,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>18</v>
       </c>
@@ -5544,7 +5547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>18</v>
       </c>
@@ -5594,7 +5597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>18</v>
       </c>
@@ -5644,7 +5647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -5694,7 +5697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>18</v>
       </c>
@@ -5744,7 +5747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -5794,7 +5797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>18</v>
       </c>
@@ -5844,7 +5847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>18</v>
       </c>
@@ -5894,7 +5897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>18</v>
       </c>
@@ -5944,7 +5947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>18</v>
       </c>
@@ -5994,7 +5997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>18</v>
       </c>
@@ -6044,7 +6047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>18</v>
       </c>
@@ -6094,7 +6097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>18</v>
       </c>
@@ -6144,7 +6147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -6194,7 +6197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>18</v>
       </c>
@@ -6244,7 +6247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>18</v>
       </c>
@@ -6294,7 +6297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>18</v>
       </c>
@@ -6344,7 +6347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -6394,7 +6397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -6444,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -6494,7 +6497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -6544,7 +6547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -6594,7 +6597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -6644,7 +6647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>14</v>
       </c>
@@ -6694,7 +6697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>14</v>
       </c>
@@ -6744,7 +6747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>14</v>
       </c>
@@ -6794,7 +6797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>14</v>
       </c>
@@ -6844,7 +6847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>14</v>
       </c>
@@ -6894,7 +6897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>14</v>
       </c>
@@ -6944,7 +6947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>14</v>
       </c>
@@ -6994,7 +6997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>14</v>
       </c>
@@ -7044,7 +7047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>14</v>
       </c>
@@ -7094,7 +7097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>14</v>
       </c>
@@ -7144,7 +7147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>14</v>
       </c>
@@ -7194,7 +7197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>14</v>
       </c>
@@ -7244,7 +7247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>14</v>
       </c>
@@ -7294,7 +7297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>14</v>
       </c>
@@ -7344,7 +7347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>14</v>
       </c>
@@ -7394,7 +7397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>14</v>
       </c>
@@ -7444,7 +7447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>14</v>
       </c>
@@ -7494,7 +7497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>14</v>
       </c>
@@ -7544,7 +7547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>14</v>
       </c>
@@ -7594,7 +7597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>14</v>
       </c>
@@ -7644,7 +7647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>14</v>
       </c>
@@ -7694,7 +7697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>14</v>
       </c>
@@ -7744,7 +7747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>14</v>
       </c>
@@ -7794,7 +7797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>14</v>
       </c>
@@ -7844,7 +7847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>14</v>
       </c>
@@ -7894,7 +7897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>14</v>
       </c>
@@ -7944,7 +7947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>14</v>
       </c>
@@ -7994,7 +7997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>14</v>
       </c>
@@ -8044,7 +8047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>14</v>
       </c>
@@ -8094,7 +8097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>14</v>
       </c>
@@ -8144,7 +8147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>14</v>
       </c>
@@ -8192,6 +8195,1506 @@
       </c>
       <c r="P155">
         <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>14</v>
+      </c>
+      <c r="B156" t="s">
+        <v>22</v>
+      </c>
+      <c r="C156">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="D156">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="E156">
+        <v>2</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
+      </c>
+      <c r="H156">
+        <v>5</v>
+      </c>
+      <c r="I156">
+        <v>2</v>
+      </c>
+      <c r="J156">
+        <v>3</v>
+      </c>
+      <c r="K156">
+        <v>3</v>
+      </c>
+      <c r="L156">
+        <v>2</v>
+      </c>
+      <c r="M156">
+        <v>1</v>
+      </c>
+      <c r="N156">
+        <v>1</v>
+      </c>
+      <c r="O156">
+        <v>0</v>
+      </c>
+      <c r="P156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>14</v>
+      </c>
+      <c r="B157" t="s">
+        <v>22</v>
+      </c>
+      <c r="C157">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="D157">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="E157">
+        <v>2</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
+      </c>
+      <c r="G157">
+        <v>1</v>
+      </c>
+      <c r="H157">
+        <v>5</v>
+      </c>
+      <c r="I157">
+        <v>2</v>
+      </c>
+      <c r="J157">
+        <v>3</v>
+      </c>
+      <c r="K157">
+        <v>3</v>
+      </c>
+      <c r="L157">
+        <v>2</v>
+      </c>
+      <c r="M157">
+        <v>1</v>
+      </c>
+      <c r="N157">
+        <v>1</v>
+      </c>
+      <c r="O157">
+        <v>0</v>
+      </c>
+      <c r="P157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>14</v>
+      </c>
+      <c r="B158" t="s">
+        <v>22</v>
+      </c>
+      <c r="C158">
+        <v>0.1</v>
+      </c>
+      <c r="D158">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="E158">
+        <v>2</v>
+      </c>
+      <c r="F158">
+        <v>1</v>
+      </c>
+      <c r="G158">
+        <v>1</v>
+      </c>
+      <c r="H158">
+        <v>5</v>
+      </c>
+      <c r="I158">
+        <v>2</v>
+      </c>
+      <c r="J158">
+        <v>3</v>
+      </c>
+      <c r="K158">
+        <v>3</v>
+      </c>
+      <c r="L158">
+        <v>2</v>
+      </c>
+      <c r="M158">
+        <v>1</v>
+      </c>
+      <c r="N158">
+        <v>1</v>
+      </c>
+      <c r="O158">
+        <v>0</v>
+      </c>
+      <c r="P158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>14</v>
+      </c>
+      <c r="B159" t="s">
+        <v>22</v>
+      </c>
+      <c r="C159">
+        <v>0.1333</v>
+      </c>
+      <c r="D159">
+        <v>0.1333</v>
+      </c>
+      <c r="E159">
+        <v>2</v>
+      </c>
+      <c r="F159">
+        <v>1</v>
+      </c>
+      <c r="G159">
+        <v>1</v>
+      </c>
+      <c r="H159">
+        <v>5</v>
+      </c>
+      <c r="I159">
+        <v>2</v>
+      </c>
+      <c r="J159">
+        <v>3</v>
+      </c>
+      <c r="K159">
+        <v>3</v>
+      </c>
+      <c r="L159">
+        <v>2</v>
+      </c>
+      <c r="M159">
+        <v>1</v>
+      </c>
+      <c r="N159">
+        <v>3</v>
+      </c>
+      <c r="O159">
+        <v>0</v>
+      </c>
+      <c r="P159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>14</v>
+      </c>
+      <c r="B160" t="s">
+        <v>22</v>
+      </c>
+      <c r="C160">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="D160">
+        <v>0.1333</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>1</v>
+      </c>
+      <c r="G160">
+        <v>3</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>2</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+      <c r="K160">
+        <v>3</v>
+      </c>
+      <c r="L160">
+        <v>4</v>
+      </c>
+      <c r="M160">
+        <v>1</v>
+      </c>
+      <c r="N160">
+        <v>5</v>
+      </c>
+      <c r="O160">
+        <v>0</v>
+      </c>
+      <c r="P160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>14</v>
+      </c>
+      <c r="B161" t="s">
+        <v>22</v>
+      </c>
+      <c r="C161">
+        <v>0.2</v>
+      </c>
+      <c r="D161">
+        <v>0.2</v>
+      </c>
+      <c r="E161">
+        <v>2</v>
+      </c>
+      <c r="F161">
+        <v>2</v>
+      </c>
+      <c r="G161">
+        <v>3</v>
+      </c>
+      <c r="H161">
+        <v>5</v>
+      </c>
+      <c r="I161">
+        <v>4</v>
+      </c>
+      <c r="J161">
+        <v>5</v>
+      </c>
+      <c r="K161">
+        <v>3</v>
+      </c>
+      <c r="L161">
+        <v>4</v>
+      </c>
+      <c r="M161">
+        <v>1</v>
+      </c>
+      <c r="N161">
+        <v>3</v>
+      </c>
+      <c r="O161">
+        <v>0</v>
+      </c>
+      <c r="P161">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>14</v>
+      </c>
+      <c r="B162" t="s">
+        <v>22</v>
+      </c>
+      <c r="C162">
+        <v>0.23330000000000001</v>
+      </c>
+      <c r="D162">
+        <v>0.2</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>2</v>
+      </c>
+      <c r="G162">
+        <v>3</v>
+      </c>
+      <c r="H162">
+        <v>5</v>
+      </c>
+      <c r="I162">
+        <v>4</v>
+      </c>
+      <c r="J162">
+        <v>0</v>
+      </c>
+      <c r="K162">
+        <v>5</v>
+      </c>
+      <c r="L162">
+        <v>4</v>
+      </c>
+      <c r="M162">
+        <v>3</v>
+      </c>
+      <c r="N162">
+        <v>3</v>
+      </c>
+      <c r="O162">
+        <v>0</v>
+      </c>
+      <c r="P162">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>14</v>
+      </c>
+      <c r="B163" t="s">
+        <v>22</v>
+      </c>
+      <c r="C163">
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="D163">
+        <v>0.2</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+      <c r="G163">
+        <v>3</v>
+      </c>
+      <c r="H163">
+        <v>5</v>
+      </c>
+      <c r="I163">
+        <v>5</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+      <c r="K163">
+        <v>0</v>
+      </c>
+      <c r="L163">
+        <v>4</v>
+      </c>
+      <c r="M163">
+        <v>3</v>
+      </c>
+      <c r="N163">
+        <v>0</v>
+      </c>
+      <c r="O163">
+        <v>0</v>
+      </c>
+      <c r="P163">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>14</v>
+      </c>
+      <c r="B164" t="s">
+        <v>22</v>
+      </c>
+      <c r="C164">
+        <v>0.3</v>
+      </c>
+      <c r="D164">
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="E164">
+        <v>2</v>
+      </c>
+      <c r="F164">
+        <v>2</v>
+      </c>
+      <c r="G164">
+        <v>3</v>
+      </c>
+      <c r="H164">
+        <v>5</v>
+      </c>
+      <c r="I164">
+        <v>4</v>
+      </c>
+      <c r="J164">
+        <v>5</v>
+      </c>
+      <c r="K164">
+        <v>5</v>
+      </c>
+      <c r="L164">
+        <v>4</v>
+      </c>
+      <c r="M164">
+        <v>3</v>
+      </c>
+      <c r="N164">
+        <v>3</v>
+      </c>
+      <c r="O164">
+        <v>0</v>
+      </c>
+      <c r="P164">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>14</v>
+      </c>
+      <c r="B165" t="s">
+        <v>22</v>
+      </c>
+      <c r="C165">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="D165">
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="G165">
+        <v>3</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+      <c r="I165">
+        <v>0</v>
+      </c>
+      <c r="J165">
+        <v>5</v>
+      </c>
+      <c r="K165">
+        <v>5</v>
+      </c>
+      <c r="L165">
+        <v>0</v>
+      </c>
+      <c r="M165">
+        <v>2</v>
+      </c>
+      <c r="N165">
+        <v>5</v>
+      </c>
+      <c r="O165">
+        <v>0</v>
+      </c>
+      <c r="P165">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>14</v>
+      </c>
+      <c r="B166" t="s">
+        <v>22</v>
+      </c>
+      <c r="C166">
+        <v>0.36670000000000003</v>
+      </c>
+      <c r="D166">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E166">
+        <v>2</v>
+      </c>
+      <c r="F166">
+        <v>4</v>
+      </c>
+      <c r="G166">
+        <v>3</v>
+      </c>
+      <c r="H166">
+        <v>5</v>
+      </c>
+      <c r="I166">
+        <v>0</v>
+      </c>
+      <c r="J166">
+        <v>5</v>
+      </c>
+      <c r="K166">
+        <v>5</v>
+      </c>
+      <c r="L166">
+        <v>2</v>
+      </c>
+      <c r="M166">
+        <v>3</v>
+      </c>
+      <c r="N166">
+        <v>4</v>
+      </c>
+      <c r="O166">
+        <v>0</v>
+      </c>
+      <c r="P166">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>14</v>
+      </c>
+      <c r="B167" t="s">
+        <v>22</v>
+      </c>
+      <c r="C167">
+        <v>0.4</v>
+      </c>
+      <c r="D167">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E167">
+        <v>4</v>
+      </c>
+      <c r="F167">
+        <v>4</v>
+      </c>
+      <c r="G167">
+        <v>3</v>
+      </c>
+      <c r="H167">
+        <v>5</v>
+      </c>
+      <c r="I167">
+        <v>0</v>
+      </c>
+      <c r="J167">
+        <v>5</v>
+      </c>
+      <c r="K167">
+        <v>5</v>
+      </c>
+      <c r="L167">
+        <v>5</v>
+      </c>
+      <c r="M167">
+        <v>3</v>
+      </c>
+      <c r="N167">
+        <v>4</v>
+      </c>
+      <c r="O167">
+        <v>0</v>
+      </c>
+      <c r="P167">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>14</v>
+      </c>
+      <c r="B168" t="s">
+        <v>22</v>
+      </c>
+      <c r="C168">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="D168">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E168">
+        <v>5</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168">
+        <v>3</v>
+      </c>
+      <c r="H168">
+        <v>5</v>
+      </c>
+      <c r="I168">
+        <v>0</v>
+      </c>
+      <c r="J168">
+        <v>0</v>
+      </c>
+      <c r="K168">
+        <v>5</v>
+      </c>
+      <c r="L168">
+        <v>5</v>
+      </c>
+      <c r="M168">
+        <v>3</v>
+      </c>
+      <c r="N168">
+        <v>0</v>
+      </c>
+      <c r="O168">
+        <v>0</v>
+      </c>
+      <c r="P168">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>14</v>
+      </c>
+      <c r="B169" t="s">
+        <v>22</v>
+      </c>
+      <c r="C169">
+        <v>0.4667</v>
+      </c>
+      <c r="D169">
+        <v>0.4</v>
+      </c>
+      <c r="E169">
+        <v>2</v>
+      </c>
+      <c r="F169">
+        <v>4</v>
+      </c>
+      <c r="G169">
+        <v>3</v>
+      </c>
+      <c r="H169">
+        <v>5</v>
+      </c>
+      <c r="I169">
+        <v>0</v>
+      </c>
+      <c r="J169">
+        <v>5</v>
+      </c>
+      <c r="K169">
+        <v>5</v>
+      </c>
+      <c r="L169">
+        <v>2</v>
+      </c>
+      <c r="M169">
+        <v>3</v>
+      </c>
+      <c r="N169">
+        <v>0</v>
+      </c>
+      <c r="O169">
+        <v>0</v>
+      </c>
+      <c r="P169">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>14</v>
+      </c>
+      <c r="B170" t="s">
+        <v>22</v>
+      </c>
+      <c r="C170">
+        <v>0.5</v>
+      </c>
+      <c r="D170">
+        <v>0.4</v>
+      </c>
+      <c r="E170">
+        <v>4</v>
+      </c>
+      <c r="F170">
+        <v>4</v>
+      </c>
+      <c r="G170">
+        <v>3</v>
+      </c>
+      <c r="H170">
+        <v>5</v>
+      </c>
+      <c r="I170">
+        <v>0</v>
+      </c>
+      <c r="J170">
+        <v>5</v>
+      </c>
+      <c r="K170">
+        <v>5</v>
+      </c>
+      <c r="L170">
+        <v>5</v>
+      </c>
+      <c r="M170">
+        <v>2</v>
+      </c>
+      <c r="N170">
+        <v>5</v>
+      </c>
+      <c r="O170">
+        <v>0</v>
+      </c>
+      <c r="P170">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>14</v>
+      </c>
+      <c r="B171" t="s">
+        <v>22</v>
+      </c>
+      <c r="C171">
+        <v>0.5333</v>
+      </c>
+      <c r="D171">
+        <v>0.4</v>
+      </c>
+      <c r="E171">
+        <v>5</v>
+      </c>
+      <c r="F171">
+        <v>4</v>
+      </c>
+      <c r="G171">
+        <v>3</v>
+      </c>
+      <c r="H171">
+        <v>0</v>
+      </c>
+      <c r="I171">
+        <v>0</v>
+      </c>
+      <c r="J171">
+        <v>0</v>
+      </c>
+      <c r="K171">
+        <v>0</v>
+      </c>
+      <c r="L171">
+        <v>0</v>
+      </c>
+      <c r="M171">
+        <v>2</v>
+      </c>
+      <c r="N171">
+        <v>0</v>
+      </c>
+      <c r="O171">
+        <v>0</v>
+      </c>
+      <c r="P171">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>14</v>
+      </c>
+      <c r="B172" t="s">
+        <v>22</v>
+      </c>
+      <c r="C172">
+        <v>0.56669999999999998</v>
+      </c>
+      <c r="D172">
+        <v>0.4667</v>
+      </c>
+      <c r="E172">
+        <v>5</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+      <c r="G172">
+        <v>2</v>
+      </c>
+      <c r="H172">
+        <v>0</v>
+      </c>
+      <c r="I172">
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+      <c r="K172">
+        <v>0</v>
+      </c>
+      <c r="L172">
+        <v>0</v>
+      </c>
+      <c r="M172">
+        <v>0</v>
+      </c>
+      <c r="N172">
+        <v>0</v>
+      </c>
+      <c r="O172">
+        <v>0</v>
+      </c>
+      <c r="P172">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>14</v>
+      </c>
+      <c r="B173" t="s">
+        <v>22</v>
+      </c>
+      <c r="C173">
+        <v>0.6</v>
+      </c>
+      <c r="D173">
+        <v>0.5333</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+      <c r="G173">
+        <v>4</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+      <c r="I173">
+        <v>0</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
+      </c>
+      <c r="K173">
+        <v>0</v>
+      </c>
+      <c r="L173">
+        <v>0</v>
+      </c>
+      <c r="M173">
+        <v>0</v>
+      </c>
+      <c r="N173">
+        <v>0</v>
+      </c>
+      <c r="O173">
+        <v>0</v>
+      </c>
+      <c r="P173">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>14</v>
+      </c>
+      <c r="B174" t="s">
+        <v>22</v>
+      </c>
+      <c r="C174">
+        <v>0.63329999999999997</v>
+      </c>
+      <c r="D174">
+        <v>0.6</v>
+      </c>
+      <c r="E174">
+        <v>4</v>
+      </c>
+      <c r="F174">
+        <v>4</v>
+      </c>
+      <c r="G174">
+        <v>2</v>
+      </c>
+      <c r="H174">
+        <v>0</v>
+      </c>
+      <c r="I174">
+        <v>5</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+      <c r="K174">
+        <v>0</v>
+      </c>
+      <c r="L174">
+        <v>5</v>
+      </c>
+      <c r="M174">
+        <v>3</v>
+      </c>
+      <c r="N174">
+        <v>0</v>
+      </c>
+      <c r="O174">
+        <v>0</v>
+      </c>
+      <c r="P174">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>14</v>
+      </c>
+      <c r="B175" t="s">
+        <v>22</v>
+      </c>
+      <c r="C175">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="D175">
+        <v>0.6</v>
+      </c>
+      <c r="E175">
+        <v>5</v>
+      </c>
+      <c r="F175">
+        <v>4</v>
+      </c>
+      <c r="G175">
+        <v>2</v>
+      </c>
+      <c r="H175">
+        <v>0</v>
+      </c>
+      <c r="I175">
+        <v>5</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
+      </c>
+      <c r="K175">
+        <v>0</v>
+      </c>
+      <c r="L175">
+        <v>5</v>
+      </c>
+      <c r="M175">
+        <v>3</v>
+      </c>
+      <c r="N175">
+        <v>0</v>
+      </c>
+      <c r="O175">
+        <v>0</v>
+      </c>
+      <c r="P175">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>14</v>
+      </c>
+      <c r="B176" t="s">
+        <v>22</v>
+      </c>
+      <c r="C176">
+        <v>0.7</v>
+      </c>
+      <c r="D176">
+        <v>0.6</v>
+      </c>
+      <c r="E176">
+        <v>5</v>
+      </c>
+      <c r="F176">
+        <v>5</v>
+      </c>
+      <c r="G176">
+        <v>5</v>
+      </c>
+      <c r="H176">
+        <v>0</v>
+      </c>
+      <c r="I176">
+        <v>5</v>
+      </c>
+      <c r="J176">
+        <v>0</v>
+      </c>
+      <c r="K176">
+        <v>0</v>
+      </c>
+      <c r="L176">
+        <v>0</v>
+      </c>
+      <c r="M176">
+        <v>3</v>
+      </c>
+      <c r="N176">
+        <v>0</v>
+      </c>
+      <c r="O176">
+        <v>0</v>
+      </c>
+      <c r="P176">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>14</v>
+      </c>
+      <c r="B177" t="s">
+        <v>22</v>
+      </c>
+      <c r="C177">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="D177">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="G177">
+        <v>5</v>
+      </c>
+      <c r="H177">
+        <v>0</v>
+      </c>
+      <c r="I177">
+        <v>0</v>
+      </c>
+      <c r="J177">
+        <v>0</v>
+      </c>
+      <c r="K177">
+        <v>0</v>
+      </c>
+      <c r="L177">
+        <v>0</v>
+      </c>
+      <c r="M177">
+        <v>0</v>
+      </c>
+      <c r="N177">
+        <v>0</v>
+      </c>
+      <c r="O177">
+        <v>0</v>
+      </c>
+      <c r="P177">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>14</v>
+      </c>
+      <c r="B178" t="s">
+        <v>22</v>
+      </c>
+      <c r="C178">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="D178">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="G178">
+        <v>5</v>
+      </c>
+      <c r="H178">
+        <v>0</v>
+      </c>
+      <c r="I178">
+        <v>0</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+      <c r="K178">
+        <v>0</v>
+      </c>
+      <c r="L178">
+        <v>0</v>
+      </c>
+      <c r="M178">
+        <v>0</v>
+      </c>
+      <c r="N178">
+        <v>0</v>
+      </c>
+      <c r="O178">
+        <v>0</v>
+      </c>
+      <c r="P178">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>14</v>
+      </c>
+      <c r="B179" t="s">
+        <v>22</v>
+      </c>
+      <c r="C179">
+        <v>0.8</v>
+      </c>
+      <c r="D179">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="G179">
+        <v>5</v>
+      </c>
+      <c r="H179">
+        <v>0</v>
+      </c>
+      <c r="I179">
+        <v>0</v>
+      </c>
+      <c r="J179">
+        <v>0</v>
+      </c>
+      <c r="K179">
+        <v>0</v>
+      </c>
+      <c r="L179">
+        <v>0</v>
+      </c>
+      <c r="M179">
+        <v>0</v>
+      </c>
+      <c r="N179">
+        <v>0</v>
+      </c>
+      <c r="O179">
+        <v>0</v>
+      </c>
+      <c r="P179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>14</v>
+      </c>
+      <c r="B180" t="s">
+        <v>22</v>
+      </c>
+      <c r="C180">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="D180">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="G180">
+        <v>5</v>
+      </c>
+      <c r="H180">
+        <v>0</v>
+      </c>
+      <c r="I180">
+        <v>0</v>
+      </c>
+      <c r="J180">
+        <v>0</v>
+      </c>
+      <c r="K180">
+        <v>0</v>
+      </c>
+      <c r="L180">
+        <v>0</v>
+      </c>
+      <c r="M180">
+        <v>0</v>
+      </c>
+      <c r="N180">
+        <v>0</v>
+      </c>
+      <c r="O180">
+        <v>0</v>
+      </c>
+      <c r="P180">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>14</v>
+      </c>
+      <c r="B181" t="s">
+        <v>22</v>
+      </c>
+      <c r="C181">
+        <v>0.86670000000000003</v>
+      </c>
+      <c r="D181">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+      <c r="G181">
+        <v>5</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181">
+        <v>0</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+      <c r="K181">
+        <v>0</v>
+      </c>
+      <c r="L181">
+        <v>0</v>
+      </c>
+      <c r="M181">
+        <v>0</v>
+      </c>
+      <c r="N181">
+        <v>0</v>
+      </c>
+      <c r="O181">
+        <v>0</v>
+      </c>
+      <c r="P181">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>14</v>
+      </c>
+      <c r="B182" t="s">
+        <v>22</v>
+      </c>
+      <c r="C182">
+        <v>0.9</v>
+      </c>
+      <c r="D182">
+        <v>0.8</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182">
+        <v>5</v>
+      </c>
+      <c r="H182">
+        <v>0</v>
+      </c>
+      <c r="I182">
+        <v>0</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+      <c r="K182">
+        <v>0</v>
+      </c>
+      <c r="L182">
+        <v>0</v>
+      </c>
+      <c r="M182">
+        <v>0</v>
+      </c>
+      <c r="N182">
+        <v>0</v>
+      </c>
+      <c r="O182">
+        <v>0</v>
+      </c>
+      <c r="P182">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>14</v>
+      </c>
+      <c r="B183" t="s">
+        <v>22</v>
+      </c>
+      <c r="C183">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="D183">
+        <v>0.86670000000000003</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183">
+        <v>5</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>0</v>
+      </c>
+      <c r="J183">
+        <v>0</v>
+      </c>
+      <c r="K183">
+        <v>0</v>
+      </c>
+      <c r="L183">
+        <v>0</v>
+      </c>
+      <c r="M183">
+        <v>0</v>
+      </c>
+      <c r="N183">
+        <v>0</v>
+      </c>
+      <c r="O183">
+        <v>0</v>
+      </c>
+      <c r="P183">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>14</v>
+      </c>
+      <c r="B184" t="s">
+        <v>22</v>
+      </c>
+      <c r="C184">
+        <v>0.9667</v>
+      </c>
+      <c r="D184">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184">
+        <v>5</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
+      </c>
+      <c r="I184">
+        <v>0</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184">
+        <v>0</v>
+      </c>
+      <c r="L184">
+        <v>0</v>
+      </c>
+      <c r="M184">
+        <v>5</v>
+      </c>
+      <c r="N184">
+        <v>0</v>
+      </c>
+      <c r="O184">
+        <v>0</v>
+      </c>
+      <c r="P184">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>14</v>
+      </c>
+      <c r="B185" t="s">
+        <v>22</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+      <c r="I185">
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+      <c r="K185">
+        <v>0</v>
+      </c>
+      <c r="L185">
+        <v>0</v>
+      </c>
+      <c r="M185">
+        <v>0</v>
+      </c>
+      <c r="N185">
+        <v>0</v>
+      </c>
+      <c r="O185">
+        <v>0</v>
+      </c>
+      <c r="P185">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added stats func and new conduit data
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanu\OneDrive\Projects\ПМЖ\2024-2025, 7М\8M_Spec_Mat_Analyze\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanu\OneDrive\Projects\ПМЖ\2024-2025, 7М\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1AE08A5-E4DB-44FB-972B-DC78DBE3EB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F9E0946-9458-44B4-8056-39DC851CA82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="problems" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="24">
   <si>
     <t>Тема</t>
   </si>
@@ -92,19 +92,22 @@
     <t>Правило умножения</t>
   </si>
   <si>
+    <t>Сочетания</t>
+  </si>
+  <si>
     <t>Алгоритм Евклида</t>
   </si>
   <si>
     <t>Сравнение по модулю</t>
   </si>
   <si>
-    <t>Сочетания-1</t>
+    <t>Диофантовы уравнения</t>
   </si>
   <si>
-    <t>Сочетания-2</t>
+    <t>Графы</t>
   </si>
   <si>
-    <t>Сочетания-3</t>
+    <t>Графы-1</t>
   </si>
 </sst>
 </file>
@@ -442,18 +445,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N185"/>
+  <dimension ref="A1:N237"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="G242" sqref="G242"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="14" width="12.6640625" customWidth="1"/>
+    <col min="3" max="14" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -541,7 +544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -585,7 +588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -629,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -673,7 +676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -717,7 +720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -761,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -805,7 +808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -849,7 +852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -893,7 +896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -937,7 +940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -981,7 +984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1905,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1993,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -2213,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -2345,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -2389,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -2433,7 +2436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -2521,7 +2524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -2565,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2609,7 +2612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -2741,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2785,12 +2788,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2829,12 +2832,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2873,12 +2876,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -2917,12 +2920,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -2961,12 +2964,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -3005,12 +3008,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -3049,12 +3052,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -3093,12 +3096,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -3137,12 +3140,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -3181,12 +3184,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C63">
         <v>2</v>
@@ -3225,12 +3228,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C64">
         <v>4</v>
@@ -3269,12 +3272,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -3313,12 +3316,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -3357,12 +3360,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C67">
         <v>2</v>
@@ -3401,12 +3404,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C68">
         <v>2</v>
@@ -3445,12 +3448,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C69">
         <v>2</v>
@@ -3489,12 +3492,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -3533,12 +3536,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C71">
         <v>2</v>
@@ -3577,12 +3580,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C72">
         <v>2</v>
@@ -3621,12 +3624,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -3665,12 +3668,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -3709,12 +3712,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C75">
         <v>4</v>
@@ -3753,12 +3756,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -3797,12 +3800,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C77">
         <v>3</v>
@@ -3841,12 +3844,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C78">
         <v>4</v>
@@ -3885,12 +3888,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -3929,12 +3932,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -3973,12 +3976,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -4017,12 +4020,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4061,12 +4064,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -4105,12 +4108,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -4149,12 +4152,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -4193,12 +4196,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>16</v>
       </c>
       <c r="B86" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C86">
         <v>3</v>
@@ -4237,12 +4240,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C87">
         <v>4</v>
@@ -4281,12 +4284,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -4325,12 +4328,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>16</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C89">
         <v>3</v>
@@ -4369,12 +4372,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C90">
         <v>3</v>
@@ -4413,12 +4416,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C91">
         <v>3</v>
@@ -4457,12 +4460,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -4501,12 +4504,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
       <c r="B93" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C93">
         <v>4</v>
@@ -4545,12 +4548,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>16</v>
       </c>
       <c r="B94" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -4589,12 +4592,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -4633,12 +4636,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>16</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C96">
         <v>4</v>
@@ -4677,12 +4680,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>16</v>
       </c>
       <c r="B97" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C97">
         <v>3</v>
@@ -4721,12 +4724,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>16</v>
       </c>
       <c r="B98" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C98">
         <v>4</v>
@@ -4765,12 +4768,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -4809,12 +4812,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
       <c r="B100" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -4853,12 +4856,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -4897,12 +4900,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
       <c r="B102" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -4941,12 +4944,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -4985,12 +4988,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>16</v>
       </c>
       <c r="B104" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -5029,12 +5032,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C105">
         <v>5</v>
@@ -5073,12 +5076,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>16</v>
       </c>
       <c r="B106" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C106">
         <v>5</v>
@@ -5117,12 +5120,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>16</v>
       </c>
       <c r="B107" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -5161,12 +5164,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>16</v>
       </c>
       <c r="B108" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -5205,12 +5208,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>16</v>
       </c>
       <c r="B109" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -5249,12 +5252,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
       <c r="B110" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C110">
         <v>5</v>
@@ -5293,12 +5296,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>16</v>
       </c>
       <c r="B111" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C111">
         <v>5</v>
@@ -5337,12 +5340,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>16</v>
       </c>
       <c r="B112" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C112">
         <v>5</v>
@@ -5381,12 +5384,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>16</v>
       </c>
       <c r="B113" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C113">
         <v>5</v>
@@ -5425,12 +5428,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>16</v>
       </c>
       <c r="B114" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C114">
         <v>5</v>
@@ -5469,12 +5472,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>16</v>
       </c>
       <c r="B115" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C115">
         <v>5</v>
@@ -5513,12 +5516,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>16</v>
       </c>
       <c r="B116" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C116">
         <v>5</v>
@@ -5557,12 +5560,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>16</v>
       </c>
       <c r="B117" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C117">
         <v>5</v>
@@ -5601,12 +5604,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>16</v>
       </c>
       <c r="B118" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C118">
         <v>5</v>
@@ -5645,12 +5648,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>16</v>
       </c>
       <c r="B119" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C119">
         <v>5</v>
@@ -5689,12 +5692,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>16</v>
       </c>
       <c r="B120" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -5733,12 +5736,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>16</v>
       </c>
       <c r="B121" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -5777,12 +5780,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>16</v>
       </c>
       <c r="B122" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -5821,12 +5824,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>16</v>
       </c>
       <c r="B123" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -5865,12 +5868,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>16</v>
       </c>
       <c r="B124" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -5909,12 +5912,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>14</v>
       </c>
       <c r="B125" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -5953,12 +5956,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>14</v>
       </c>
       <c r="B126" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -5997,12 +6000,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>14</v>
       </c>
       <c r="B127" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -6041,12 +6044,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>14</v>
       </c>
       <c r="B128" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -6085,12 +6088,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>14</v>
       </c>
       <c r="B129" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C129">
         <v>4</v>
@@ -6129,12 +6132,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>14</v>
       </c>
       <c r="B130" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -6173,12 +6176,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>14</v>
       </c>
       <c r="B131" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C131">
         <v>5</v>
@@ -6217,12 +6220,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>14</v>
       </c>
       <c r="B132" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C132">
         <v>5</v>
@@ -6261,12 +6264,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>14</v>
       </c>
       <c r="B133" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C133">
         <v>5</v>
@@ -6305,12 +6308,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>14</v>
       </c>
       <c r="B134" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C134">
         <v>7</v>
@@ -6349,12 +6352,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>14</v>
       </c>
       <c r="B135" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C135">
         <v>4</v>
@@ -6393,12 +6396,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>14</v>
       </c>
       <c r="B136" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -6437,12 +6440,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>14</v>
       </c>
       <c r="B137" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -6481,12 +6484,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>14</v>
       </c>
       <c r="B138" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -6525,12 +6528,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>14</v>
       </c>
       <c r="B139" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -6569,12 +6572,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>14</v>
       </c>
       <c r="B140" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -6613,12 +6616,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>14</v>
       </c>
       <c r="B141" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -6657,12 +6660,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>14</v>
       </c>
       <c r="B142" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C142">
         <v>4</v>
@@ -6701,12 +6704,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>14</v>
       </c>
       <c r="B143" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C143">
         <v>4</v>
@@ -6745,12 +6748,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>14</v>
       </c>
       <c r="B144" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C144">
         <v>6</v>
@@ -6789,12 +6792,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>14</v>
       </c>
       <c r="B145" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C145">
         <v>6</v>
@@ -6833,12 +6836,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>14</v>
       </c>
       <c r="B146" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C146">
         <v>4</v>
@@ -6877,12 +6880,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>14</v>
       </c>
       <c r="B147" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C147">
         <v>5</v>
@@ -6921,12 +6924,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>14</v>
       </c>
       <c r="B148" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C148">
         <v>6</v>
@@ -6965,12 +6968,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>14</v>
       </c>
       <c r="B149" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C149">
         <v>6</v>
@@ -7009,12 +7012,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>14</v>
       </c>
       <c r="B150" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C150">
         <v>6</v>
@@ -7053,12 +7056,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>14</v>
       </c>
       <c r="B151" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C151">
         <v>6</v>
@@ -7097,12 +7100,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>14</v>
       </c>
       <c r="B152" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C152">
         <v>7</v>
@@ -7141,12 +7144,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>14</v>
       </c>
       <c r="B153" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C153">
         <v>7</v>
@@ -7185,12 +7188,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>14</v>
       </c>
       <c r="B154" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C154">
         <v>7</v>
@@ -7229,12 +7232,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>14</v>
       </c>
       <c r="B155" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C155">
         <v>7</v>
@@ -7273,12 +7276,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>14</v>
       </c>
       <c r="B156" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C156">
         <v>2</v>
@@ -7317,12 +7320,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>14</v>
       </c>
       <c r="B157" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C157">
         <v>2</v>
@@ -7361,12 +7364,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>14</v>
       </c>
       <c r="B158" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C158">
         <v>2</v>
@@ -7405,12 +7408,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>14</v>
       </c>
       <c r="B159" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C159">
         <v>2</v>
@@ -7449,12 +7452,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>14</v>
       </c>
       <c r="B160" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -7493,12 +7496,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>14</v>
       </c>
       <c r="B161" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C161">
         <v>2</v>
@@ -7537,12 +7540,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>14</v>
       </c>
       <c r="B162" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -7581,12 +7584,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>14</v>
       </c>
       <c r="B163" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -7625,12 +7628,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>14</v>
       </c>
       <c r="B164" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C164">
         <v>2</v>
@@ -7669,12 +7672,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>14</v>
       </c>
       <c r="B165" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -7713,12 +7716,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>14</v>
       </c>
       <c r="B166" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C166">
         <v>2</v>
@@ -7757,12 +7760,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>14</v>
       </c>
       <c r="B167" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C167">
         <v>4</v>
@@ -7801,12 +7804,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>14</v>
       </c>
       <c r="B168" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C168">
         <v>5</v>
@@ -7845,12 +7848,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>14</v>
       </c>
       <c r="B169" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C169">
         <v>2</v>
@@ -7889,12 +7892,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>14</v>
       </c>
       <c r="B170" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C170">
         <v>4</v>
@@ -7933,12 +7936,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>14</v>
       </c>
       <c r="B171" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C171">
         <v>5</v>
@@ -7977,12 +7980,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>14</v>
       </c>
       <c r="B172" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C172">
         <v>5</v>
@@ -8021,12 +8024,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>14</v>
       </c>
       <c r="B173" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C173">
         <v>0</v>
@@ -8065,12 +8068,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>14</v>
       </c>
       <c r="B174" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C174">
         <v>4</v>
@@ -8109,12 +8112,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>14</v>
       </c>
       <c r="B175" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C175">
         <v>5</v>
@@ -8153,12 +8156,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>14</v>
       </c>
       <c r="B176" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C176">
         <v>5</v>
@@ -8197,12 +8200,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>14</v>
       </c>
       <c r="B177" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -8241,12 +8244,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>14</v>
       </c>
       <c r="B178" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C178">
         <v>0</v>
@@ -8285,12 +8288,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>14</v>
       </c>
       <c r="B179" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -8329,12 +8332,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>14</v>
       </c>
       <c r="B180" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C180">
         <v>0</v>
@@ -8373,12 +8376,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>14</v>
       </c>
       <c r="B181" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C181">
         <v>0</v>
@@ -8417,12 +8420,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>14</v>
       </c>
       <c r="B182" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C182">
         <v>0</v>
@@ -8461,12 +8464,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>14</v>
       </c>
       <c r="B183" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C183">
         <v>0</v>
@@ -8505,12 +8508,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>14</v>
       </c>
       <c r="B184" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -8549,12 +8552,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>14</v>
       </c>
       <c r="B185" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C185">
         <v>0</v>
@@ -8591,6 +8594,2294 @@
       </c>
       <c r="N185">
         <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>14</v>
+      </c>
+      <c r="B186" t="s">
+        <v>21</v>
+      </c>
+      <c r="C186">
+        <v>4</v>
+      </c>
+      <c r="D186">
+        <v>2</v>
+      </c>
+      <c r="E186">
+        <v>1</v>
+      </c>
+      <c r="F186">
+        <v>4</v>
+      </c>
+      <c r="G186">
+        <v>6</v>
+      </c>
+      <c r="H186">
+        <v>6</v>
+      </c>
+      <c r="I186">
+        <v>4</v>
+      </c>
+      <c r="J186">
+        <v>1</v>
+      </c>
+      <c r="K186">
+        <v>3</v>
+      </c>
+      <c r="L186">
+        <v>1</v>
+      </c>
+      <c r="M186">
+        <v>6</v>
+      </c>
+      <c r="N186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>14</v>
+      </c>
+      <c r="B187" t="s">
+        <v>21</v>
+      </c>
+      <c r="C187">
+        <v>4</v>
+      </c>
+      <c r="D187">
+        <v>6</v>
+      </c>
+      <c r="E187">
+        <v>4</v>
+      </c>
+      <c r="F187">
+        <v>4</v>
+      </c>
+      <c r="G187">
+        <v>6</v>
+      </c>
+      <c r="H187">
+        <v>6</v>
+      </c>
+      <c r="I187">
+        <v>4</v>
+      </c>
+      <c r="J187">
+        <v>1</v>
+      </c>
+      <c r="K187">
+        <v>3</v>
+      </c>
+      <c r="L187">
+        <v>2</v>
+      </c>
+      <c r="M187">
+        <v>6</v>
+      </c>
+      <c r="N187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>14</v>
+      </c>
+      <c r="B188" t="s">
+        <v>21</v>
+      </c>
+      <c r="C188">
+        <v>4</v>
+      </c>
+      <c r="D188">
+        <v>6</v>
+      </c>
+      <c r="E188">
+        <v>5</v>
+      </c>
+      <c r="F188">
+        <v>4</v>
+      </c>
+      <c r="G188">
+        <v>6</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+      <c r="I188">
+        <v>4</v>
+      </c>
+      <c r="J188">
+        <v>2</v>
+      </c>
+      <c r="K188">
+        <v>3</v>
+      </c>
+      <c r="L188">
+        <v>6</v>
+      </c>
+      <c r="M188">
+        <v>6</v>
+      </c>
+      <c r="N188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>14</v>
+      </c>
+      <c r="B189" t="s">
+        <v>21</v>
+      </c>
+      <c r="C189">
+        <v>2</v>
+      </c>
+      <c r="D189">
+        <v>2</v>
+      </c>
+      <c r="E189">
+        <v>1</v>
+      </c>
+      <c r="F189">
+        <v>3</v>
+      </c>
+      <c r="G189">
+        <v>2</v>
+      </c>
+      <c r="H189">
+        <v>5</v>
+      </c>
+      <c r="I189">
+        <v>4</v>
+      </c>
+      <c r="J189">
+        <v>2</v>
+      </c>
+      <c r="K189">
+        <v>3</v>
+      </c>
+      <c r="L189">
+        <v>1</v>
+      </c>
+      <c r="M189">
+        <v>2</v>
+      </c>
+      <c r="N189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>14</v>
+      </c>
+      <c r="B190" t="s">
+        <v>21</v>
+      </c>
+      <c r="C190">
+        <v>2</v>
+      </c>
+      <c r="D190">
+        <v>2</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+      <c r="F190">
+        <v>3</v>
+      </c>
+      <c r="G190">
+        <v>3</v>
+      </c>
+      <c r="H190">
+        <v>6</v>
+      </c>
+      <c r="I190">
+        <v>4</v>
+      </c>
+      <c r="J190">
+        <v>2</v>
+      </c>
+      <c r="K190">
+        <v>3</v>
+      </c>
+      <c r="L190">
+        <v>1</v>
+      </c>
+      <c r="M190">
+        <v>2</v>
+      </c>
+      <c r="N190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>14</v>
+      </c>
+      <c r="B191" t="s">
+        <v>21</v>
+      </c>
+      <c r="C191">
+        <v>2</v>
+      </c>
+      <c r="D191">
+        <v>2</v>
+      </c>
+      <c r="E191">
+        <v>2</v>
+      </c>
+      <c r="F191">
+        <v>4</v>
+      </c>
+      <c r="G191">
+        <v>3</v>
+      </c>
+      <c r="H191">
+        <v>5</v>
+      </c>
+      <c r="I191">
+        <v>4</v>
+      </c>
+      <c r="J191">
+        <v>2</v>
+      </c>
+      <c r="K191">
+        <v>3</v>
+      </c>
+      <c r="L191">
+        <v>2</v>
+      </c>
+      <c r="M191">
+        <v>2</v>
+      </c>
+      <c r="N191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>14</v>
+      </c>
+      <c r="B192" t="s">
+        <v>21</v>
+      </c>
+      <c r="C192">
+        <v>2</v>
+      </c>
+      <c r="D192">
+        <v>2</v>
+      </c>
+      <c r="E192">
+        <v>4</v>
+      </c>
+      <c r="F192">
+        <v>4</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>0</v>
+      </c>
+      <c r="I192">
+        <v>4</v>
+      </c>
+      <c r="J192">
+        <v>2</v>
+      </c>
+      <c r="K192">
+        <v>0</v>
+      </c>
+      <c r="L192">
+        <v>2</v>
+      </c>
+      <c r="M192">
+        <v>5</v>
+      </c>
+      <c r="N192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>14</v>
+      </c>
+      <c r="B193" t="s">
+        <v>21</v>
+      </c>
+      <c r="C193">
+        <v>3</v>
+      </c>
+      <c r="D193">
+        <v>6</v>
+      </c>
+      <c r="E193">
+        <v>5</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>5</v>
+      </c>
+      <c r="I193">
+        <v>6</v>
+      </c>
+      <c r="J193">
+        <v>2</v>
+      </c>
+      <c r="K193">
+        <v>0</v>
+      </c>
+      <c r="L193">
+        <v>6</v>
+      </c>
+      <c r="M193">
+        <v>5</v>
+      </c>
+      <c r="N193">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>14</v>
+      </c>
+      <c r="B194" t="s">
+        <v>21</v>
+      </c>
+      <c r="C194">
+        <v>4</v>
+      </c>
+      <c r="D194">
+        <v>6</v>
+      </c>
+      <c r="E194">
+        <v>6</v>
+      </c>
+      <c r="F194">
+        <v>0</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
+      <c r="H194">
+        <v>0</v>
+      </c>
+      <c r="I194">
+        <v>6</v>
+      </c>
+      <c r="J194">
+        <v>2</v>
+      </c>
+      <c r="K194">
+        <v>0</v>
+      </c>
+      <c r="L194">
+        <v>6</v>
+      </c>
+      <c r="M194">
+        <v>6</v>
+      </c>
+      <c r="N194">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>14</v>
+      </c>
+      <c r="B195" t="s">
+        <v>21</v>
+      </c>
+      <c r="C195">
+        <v>4</v>
+      </c>
+      <c r="D195">
+        <v>6</v>
+      </c>
+      <c r="E195">
+        <v>6</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195">
+        <v>0</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="I195">
+        <v>6</v>
+      </c>
+      <c r="J195">
+        <v>2</v>
+      </c>
+      <c r="K195">
+        <v>0</v>
+      </c>
+      <c r="L195">
+        <v>6</v>
+      </c>
+      <c r="M195">
+        <v>6</v>
+      </c>
+      <c r="N195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>14</v>
+      </c>
+      <c r="B196" t="s">
+        <v>21</v>
+      </c>
+      <c r="C196">
+        <v>3</v>
+      </c>
+      <c r="D196">
+        <v>6</v>
+      </c>
+      <c r="E196">
+        <v>4</v>
+      </c>
+      <c r="F196">
+        <v>4</v>
+      </c>
+      <c r="G196">
+        <v>6</v>
+      </c>
+      <c r="H196">
+        <v>6</v>
+      </c>
+      <c r="I196">
+        <v>0</v>
+      </c>
+      <c r="J196">
+        <v>3</v>
+      </c>
+      <c r="K196">
+        <v>6</v>
+      </c>
+      <c r="L196">
+        <v>5</v>
+      </c>
+      <c r="M196">
+        <v>6</v>
+      </c>
+      <c r="N196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>14</v>
+      </c>
+      <c r="B197" t="s">
+        <v>21</v>
+      </c>
+      <c r="C197">
+        <v>3</v>
+      </c>
+      <c r="D197">
+        <v>6</v>
+      </c>
+      <c r="E197">
+        <v>2</v>
+      </c>
+      <c r="F197">
+        <v>4</v>
+      </c>
+      <c r="G197">
+        <v>6</v>
+      </c>
+      <c r="H197">
+        <v>5</v>
+      </c>
+      <c r="I197">
+        <v>0</v>
+      </c>
+      <c r="J197">
+        <v>3</v>
+      </c>
+      <c r="K197">
+        <v>0</v>
+      </c>
+      <c r="L197">
+        <v>5</v>
+      </c>
+      <c r="M197">
+        <v>5</v>
+      </c>
+      <c r="N197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>14</v>
+      </c>
+      <c r="B198" t="s">
+        <v>21</v>
+      </c>
+      <c r="C198">
+        <v>4</v>
+      </c>
+      <c r="D198">
+        <v>6</v>
+      </c>
+      <c r="E198">
+        <v>4</v>
+      </c>
+      <c r="F198">
+        <v>4</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>0</v>
+      </c>
+      <c r="I198">
+        <v>0</v>
+      </c>
+      <c r="J198">
+        <v>3</v>
+      </c>
+      <c r="K198">
+        <v>6</v>
+      </c>
+      <c r="L198">
+        <v>5</v>
+      </c>
+      <c r="M198">
+        <v>6</v>
+      </c>
+      <c r="N198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>14</v>
+      </c>
+      <c r="B199" t="s">
+        <v>21</v>
+      </c>
+      <c r="C199">
+        <v>4</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>6</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>6</v>
+      </c>
+      <c r="I199">
+        <v>0</v>
+      </c>
+      <c r="J199">
+        <v>3</v>
+      </c>
+      <c r="K199">
+        <v>0</v>
+      </c>
+      <c r="L199">
+        <v>6</v>
+      </c>
+      <c r="M199">
+        <v>6</v>
+      </c>
+      <c r="N199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>14</v>
+      </c>
+      <c r="B200" t="s">
+        <v>21</v>
+      </c>
+      <c r="C200">
+        <v>6</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>6</v>
+      </c>
+      <c r="F200">
+        <v>0</v>
+      </c>
+      <c r="G200">
+        <v>0</v>
+      </c>
+      <c r="H200">
+        <v>0</v>
+      </c>
+      <c r="I200">
+        <v>0</v>
+      </c>
+      <c r="J200">
+        <v>3</v>
+      </c>
+      <c r="K200">
+        <v>0</v>
+      </c>
+      <c r="L200">
+        <v>0</v>
+      </c>
+      <c r="M200">
+        <v>6</v>
+      </c>
+      <c r="N200">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>14</v>
+      </c>
+      <c r="B201" t="s">
+        <v>21</v>
+      </c>
+      <c r="C201">
+        <v>4</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201">
+        <v>6</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+      <c r="G201">
+        <v>0</v>
+      </c>
+      <c r="H201">
+        <v>0</v>
+      </c>
+      <c r="I201">
+        <v>0</v>
+      </c>
+      <c r="J201">
+        <v>4</v>
+      </c>
+      <c r="K201">
+        <v>0</v>
+      </c>
+      <c r="L201">
+        <v>6</v>
+      </c>
+      <c r="M201">
+        <v>6</v>
+      </c>
+      <c r="N201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>14</v>
+      </c>
+      <c r="B202" t="s">
+        <v>21</v>
+      </c>
+      <c r="C202">
+        <v>3</v>
+      </c>
+      <c r="D202">
+        <v>2</v>
+      </c>
+      <c r="E202">
+        <v>2</v>
+      </c>
+      <c r="F202">
+        <v>3</v>
+      </c>
+      <c r="G202">
+        <v>2</v>
+      </c>
+      <c r="H202">
+        <v>4</v>
+      </c>
+      <c r="I202">
+        <v>4</v>
+      </c>
+      <c r="J202">
+        <v>4</v>
+      </c>
+      <c r="K202">
+        <v>3</v>
+      </c>
+      <c r="L202">
+        <v>5</v>
+      </c>
+      <c r="M202">
+        <v>2</v>
+      </c>
+      <c r="N202">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>14</v>
+      </c>
+      <c r="B203" t="s">
+        <v>21</v>
+      </c>
+      <c r="C203">
+        <v>3</v>
+      </c>
+      <c r="D203">
+        <v>2</v>
+      </c>
+      <c r="E203">
+        <v>2</v>
+      </c>
+      <c r="F203">
+        <v>3</v>
+      </c>
+      <c r="G203">
+        <v>2</v>
+      </c>
+      <c r="H203">
+        <v>4</v>
+      </c>
+      <c r="I203">
+        <v>4</v>
+      </c>
+      <c r="J203">
+        <v>4</v>
+      </c>
+      <c r="K203">
+        <v>3</v>
+      </c>
+      <c r="L203">
+        <v>5</v>
+      </c>
+      <c r="M203">
+        <v>6</v>
+      </c>
+      <c r="N203">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>14</v>
+      </c>
+      <c r="B204" t="s">
+        <v>21</v>
+      </c>
+      <c r="C204">
+        <v>4</v>
+      </c>
+      <c r="D204">
+        <v>2</v>
+      </c>
+      <c r="E204">
+        <v>6</v>
+      </c>
+      <c r="F204">
+        <v>3</v>
+      </c>
+      <c r="G204">
+        <v>2</v>
+      </c>
+      <c r="H204">
+        <v>0</v>
+      </c>
+      <c r="I204">
+        <v>4</v>
+      </c>
+      <c r="J204">
+        <v>4</v>
+      </c>
+      <c r="K204">
+        <v>3</v>
+      </c>
+      <c r="L204">
+        <v>5</v>
+      </c>
+      <c r="M204">
+        <v>0</v>
+      </c>
+      <c r="N204">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>14</v>
+      </c>
+      <c r="B205" t="s">
+        <v>21</v>
+      </c>
+      <c r="C205">
+        <v>6</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205">
+        <v>6</v>
+      </c>
+      <c r="F205">
+        <v>0</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
+      <c r="H205">
+        <v>0</v>
+      </c>
+      <c r="I205">
+        <v>0</v>
+      </c>
+      <c r="J205">
+        <v>0</v>
+      </c>
+      <c r="K205">
+        <v>3</v>
+      </c>
+      <c r="L205">
+        <v>0</v>
+      </c>
+      <c r="M205">
+        <v>0</v>
+      </c>
+      <c r="N205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>14</v>
+      </c>
+      <c r="B206" t="s">
+        <v>21</v>
+      </c>
+      <c r="C206">
+        <v>0</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>6</v>
+      </c>
+      <c r="F206">
+        <v>0</v>
+      </c>
+      <c r="G206">
+        <v>0</v>
+      </c>
+      <c r="H206">
+        <v>0</v>
+      </c>
+      <c r="I206">
+        <v>0</v>
+      </c>
+      <c r="J206">
+        <v>0</v>
+      </c>
+      <c r="K206">
+        <v>0</v>
+      </c>
+      <c r="L206">
+        <v>0</v>
+      </c>
+      <c r="M206">
+        <v>0</v>
+      </c>
+      <c r="N206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>14</v>
+      </c>
+      <c r="B207" t="s">
+        <v>21</v>
+      </c>
+      <c r="C207">
+        <v>0</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207">
+        <v>6</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+      <c r="G207">
+        <v>0</v>
+      </c>
+      <c r="H207">
+        <v>0</v>
+      </c>
+      <c r="I207">
+        <v>0</v>
+      </c>
+      <c r="J207">
+        <v>0</v>
+      </c>
+      <c r="K207">
+        <v>0</v>
+      </c>
+      <c r="L207">
+        <v>0</v>
+      </c>
+      <c r="M207">
+        <v>0</v>
+      </c>
+      <c r="N207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>14</v>
+      </c>
+      <c r="B208" t="s">
+        <v>21</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="E208">
+        <v>0</v>
+      </c>
+      <c r="F208">
+        <v>0</v>
+      </c>
+      <c r="G208">
+        <v>0</v>
+      </c>
+      <c r="H208">
+        <v>0</v>
+      </c>
+      <c r="I208">
+        <v>0</v>
+      </c>
+      <c r="J208">
+        <v>0</v>
+      </c>
+      <c r="K208">
+        <v>0</v>
+      </c>
+      <c r="L208">
+        <v>0</v>
+      </c>
+      <c r="M208">
+        <v>0</v>
+      </c>
+      <c r="N208">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>14</v>
+      </c>
+      <c r="B209" t="s">
+        <v>21</v>
+      </c>
+      <c r="C209">
+        <v>0</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>0</v>
+      </c>
+      <c r="F209">
+        <v>0</v>
+      </c>
+      <c r="G209">
+        <v>0</v>
+      </c>
+      <c r="H209">
+        <v>0</v>
+      </c>
+      <c r="I209">
+        <v>0</v>
+      </c>
+      <c r="J209">
+        <v>0</v>
+      </c>
+      <c r="K209">
+        <v>0</v>
+      </c>
+      <c r="L209">
+        <v>0</v>
+      </c>
+      <c r="M209">
+        <v>0</v>
+      </c>
+      <c r="N209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>14</v>
+      </c>
+      <c r="B210" t="s">
+        <v>21</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>0</v>
+      </c>
+      <c r="F210">
+        <v>0</v>
+      </c>
+      <c r="G210">
+        <v>0</v>
+      </c>
+      <c r="H210">
+        <v>0</v>
+      </c>
+      <c r="I210">
+        <v>0</v>
+      </c>
+      <c r="J210">
+        <v>0</v>
+      </c>
+      <c r="K210">
+        <v>0</v>
+      </c>
+      <c r="L210">
+        <v>0</v>
+      </c>
+      <c r="M210">
+        <v>0</v>
+      </c>
+      <c r="N210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>14</v>
+      </c>
+      <c r="B211" t="s">
+        <v>21</v>
+      </c>
+      <c r="C211">
+        <v>0</v>
+      </c>
+      <c r="D211">
+        <v>0</v>
+      </c>
+      <c r="E211">
+        <v>0</v>
+      </c>
+      <c r="F211">
+        <v>0</v>
+      </c>
+      <c r="G211">
+        <v>0</v>
+      </c>
+      <c r="H211">
+        <v>0</v>
+      </c>
+      <c r="I211">
+        <v>0</v>
+      </c>
+      <c r="J211">
+        <v>0</v>
+      </c>
+      <c r="K211">
+        <v>0</v>
+      </c>
+      <c r="L211">
+        <v>0</v>
+      </c>
+      <c r="M211">
+        <v>0</v>
+      </c>
+      <c r="N211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>14</v>
+      </c>
+      <c r="B212" t="s">
+        <v>21</v>
+      </c>
+      <c r="C212">
+        <v>0</v>
+      </c>
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="E212">
+        <v>0</v>
+      </c>
+      <c r="F212">
+        <v>0</v>
+      </c>
+      <c r="G212">
+        <v>0</v>
+      </c>
+      <c r="H212">
+        <v>0</v>
+      </c>
+      <c r="I212">
+        <v>0</v>
+      </c>
+      <c r="J212">
+        <v>0</v>
+      </c>
+      <c r="K212">
+        <v>0</v>
+      </c>
+      <c r="L212">
+        <v>0</v>
+      </c>
+      <c r="M212">
+        <v>0</v>
+      </c>
+      <c r="N212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>14</v>
+      </c>
+      <c r="B213" t="s">
+        <v>21</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>0</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="G213">
+        <v>0</v>
+      </c>
+      <c r="H213">
+        <v>0</v>
+      </c>
+      <c r="I213">
+        <v>0</v>
+      </c>
+      <c r="J213">
+        <v>0</v>
+      </c>
+      <c r="K213">
+        <v>0</v>
+      </c>
+      <c r="L213">
+        <v>0</v>
+      </c>
+      <c r="M213">
+        <v>0</v>
+      </c>
+      <c r="N213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>14</v>
+      </c>
+      <c r="B214" t="s">
+        <v>21</v>
+      </c>
+      <c r="C214">
+        <v>0</v>
+      </c>
+      <c r="D214">
+        <v>0</v>
+      </c>
+      <c r="E214">
+        <v>0</v>
+      </c>
+      <c r="F214">
+        <v>0</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
+      <c r="H214">
+        <v>0</v>
+      </c>
+      <c r="I214">
+        <v>0</v>
+      </c>
+      <c r="J214">
+        <v>0</v>
+      </c>
+      <c r="K214">
+        <v>0</v>
+      </c>
+      <c r="L214">
+        <v>0</v>
+      </c>
+      <c r="M214">
+        <v>0</v>
+      </c>
+      <c r="N214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>14</v>
+      </c>
+      <c r="B215" t="s">
+        <v>21</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="E215">
+        <v>0</v>
+      </c>
+      <c r="F215">
+        <v>0</v>
+      </c>
+      <c r="G215">
+        <v>0</v>
+      </c>
+      <c r="H215">
+        <v>0</v>
+      </c>
+      <c r="I215">
+        <v>0</v>
+      </c>
+      <c r="J215">
+        <v>0</v>
+      </c>
+      <c r="K215">
+        <v>0</v>
+      </c>
+      <c r="L215">
+        <v>0</v>
+      </c>
+      <c r="M215">
+        <v>0</v>
+      </c>
+      <c r="N215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>22</v>
+      </c>
+      <c r="B216" t="s">
+        <v>23</v>
+      </c>
+      <c r="C216">
+        <v>4</v>
+      </c>
+      <c r="D216">
+        <v>1</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+      <c r="F216">
+        <v>1</v>
+      </c>
+      <c r="G216">
+        <v>1</v>
+      </c>
+      <c r="H216">
+        <v>4</v>
+      </c>
+      <c r="I216">
+        <v>2</v>
+      </c>
+      <c r="J216">
+        <v>1</v>
+      </c>
+      <c r="K216">
+        <v>1</v>
+      </c>
+      <c r="L216">
+        <v>1</v>
+      </c>
+      <c r="M216">
+        <v>2</v>
+      </c>
+      <c r="N216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>22</v>
+      </c>
+      <c r="B217" t="s">
+        <v>23</v>
+      </c>
+      <c r="C217">
+        <v>4</v>
+      </c>
+      <c r="D217">
+        <v>1</v>
+      </c>
+      <c r="E217">
+        <v>1</v>
+      </c>
+      <c r="F217">
+        <v>1</v>
+      </c>
+      <c r="G217">
+        <v>1</v>
+      </c>
+      <c r="H217">
+        <v>4</v>
+      </c>
+      <c r="I217">
+        <v>2</v>
+      </c>
+      <c r="J217">
+        <v>1</v>
+      </c>
+      <c r="K217">
+        <v>1</v>
+      </c>
+      <c r="L217">
+        <v>1</v>
+      </c>
+      <c r="M217">
+        <v>2</v>
+      </c>
+      <c r="N217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>22</v>
+      </c>
+      <c r="B218" t="s">
+        <v>23</v>
+      </c>
+      <c r="C218">
+        <v>4</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+      <c r="F218">
+        <v>1</v>
+      </c>
+      <c r="G218">
+        <v>1</v>
+      </c>
+      <c r="H218">
+        <v>4</v>
+      </c>
+      <c r="I218">
+        <v>2</v>
+      </c>
+      <c r="J218">
+        <v>1</v>
+      </c>
+      <c r="K218">
+        <v>1</v>
+      </c>
+      <c r="L218">
+        <v>1</v>
+      </c>
+      <c r="M218">
+        <v>2</v>
+      </c>
+      <c r="N218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>22</v>
+      </c>
+      <c r="B219" t="s">
+        <v>23</v>
+      </c>
+      <c r="C219">
+        <v>4</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+      <c r="E219">
+        <v>1</v>
+      </c>
+      <c r="F219">
+        <v>1</v>
+      </c>
+      <c r="G219">
+        <v>1</v>
+      </c>
+      <c r="H219">
+        <v>4</v>
+      </c>
+      <c r="I219">
+        <v>2</v>
+      </c>
+      <c r="J219">
+        <v>1</v>
+      </c>
+      <c r="K219">
+        <v>1</v>
+      </c>
+      <c r="L219">
+        <v>1</v>
+      </c>
+      <c r="M219">
+        <v>2</v>
+      </c>
+      <c r="N219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>22</v>
+      </c>
+      <c r="B220" t="s">
+        <v>23</v>
+      </c>
+      <c r="C220">
+        <v>4</v>
+      </c>
+      <c r="D220">
+        <v>1</v>
+      </c>
+      <c r="E220">
+        <v>1</v>
+      </c>
+      <c r="F220">
+        <v>1</v>
+      </c>
+      <c r="G220">
+        <v>1</v>
+      </c>
+      <c r="H220">
+        <v>4</v>
+      </c>
+      <c r="I220">
+        <v>2</v>
+      </c>
+      <c r="J220">
+        <v>1</v>
+      </c>
+      <c r="K220">
+        <v>1</v>
+      </c>
+      <c r="L220">
+        <v>1</v>
+      </c>
+      <c r="M220">
+        <v>2</v>
+      </c>
+      <c r="N220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>22</v>
+      </c>
+      <c r="B221" t="s">
+        <v>23</v>
+      </c>
+      <c r="C221">
+        <v>4</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+      <c r="E221">
+        <v>1</v>
+      </c>
+      <c r="F221">
+        <v>1</v>
+      </c>
+      <c r="G221">
+        <v>1</v>
+      </c>
+      <c r="H221">
+        <v>4</v>
+      </c>
+      <c r="I221">
+        <v>2</v>
+      </c>
+      <c r="J221">
+        <v>1</v>
+      </c>
+      <c r="K221">
+        <v>1</v>
+      </c>
+      <c r="L221">
+        <v>1</v>
+      </c>
+      <c r="M221">
+        <v>2</v>
+      </c>
+      <c r="N221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>22</v>
+      </c>
+      <c r="B222" t="s">
+        <v>23</v>
+      </c>
+      <c r="C222">
+        <v>4</v>
+      </c>
+      <c r="D222">
+        <v>2</v>
+      </c>
+      <c r="E222">
+        <v>1</v>
+      </c>
+      <c r="F222">
+        <v>1</v>
+      </c>
+      <c r="G222">
+        <v>1</v>
+      </c>
+      <c r="H222">
+        <v>4</v>
+      </c>
+      <c r="I222">
+        <v>2</v>
+      </c>
+      <c r="J222">
+        <v>1</v>
+      </c>
+      <c r="K222">
+        <v>1</v>
+      </c>
+      <c r="L222">
+        <v>1</v>
+      </c>
+      <c r="M222">
+        <v>2</v>
+      </c>
+      <c r="N222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>22</v>
+      </c>
+      <c r="B223" t="s">
+        <v>23</v>
+      </c>
+      <c r="C223">
+        <v>4</v>
+      </c>
+      <c r="D223">
+        <v>2</v>
+      </c>
+      <c r="E223">
+        <v>1</v>
+      </c>
+      <c r="F223">
+        <v>1</v>
+      </c>
+      <c r="G223">
+        <v>1</v>
+      </c>
+      <c r="H223">
+        <v>4</v>
+      </c>
+      <c r="I223">
+        <v>2</v>
+      </c>
+      <c r="J223">
+        <v>1</v>
+      </c>
+      <c r="K223">
+        <v>1</v>
+      </c>
+      <c r="L223">
+        <v>1</v>
+      </c>
+      <c r="M223">
+        <v>2</v>
+      </c>
+      <c r="N223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>22</v>
+      </c>
+      <c r="B224" t="s">
+        <v>23</v>
+      </c>
+      <c r="C224">
+        <v>4</v>
+      </c>
+      <c r="D224">
+        <v>1</v>
+      </c>
+      <c r="E224">
+        <v>2</v>
+      </c>
+      <c r="F224">
+        <v>1</v>
+      </c>
+      <c r="G224">
+        <v>1</v>
+      </c>
+      <c r="H224">
+        <v>4</v>
+      </c>
+      <c r="I224">
+        <v>2</v>
+      </c>
+      <c r="J224">
+        <v>1</v>
+      </c>
+      <c r="K224">
+        <v>1</v>
+      </c>
+      <c r="L224">
+        <v>2</v>
+      </c>
+      <c r="M224">
+        <v>3</v>
+      </c>
+      <c r="N224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>22</v>
+      </c>
+      <c r="B225" t="s">
+        <v>23</v>
+      </c>
+      <c r="C225">
+        <v>4</v>
+      </c>
+      <c r="D225">
+        <v>2</v>
+      </c>
+      <c r="E225">
+        <v>2</v>
+      </c>
+      <c r="F225">
+        <v>1</v>
+      </c>
+      <c r="G225">
+        <v>1</v>
+      </c>
+      <c r="H225">
+        <v>4</v>
+      </c>
+      <c r="I225">
+        <v>2</v>
+      </c>
+      <c r="J225">
+        <v>1</v>
+      </c>
+      <c r="K225">
+        <v>1</v>
+      </c>
+      <c r="L225">
+        <v>2</v>
+      </c>
+      <c r="M225">
+        <v>3</v>
+      </c>
+      <c r="N225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>22</v>
+      </c>
+      <c r="B226" t="s">
+        <v>23</v>
+      </c>
+      <c r="C226">
+        <v>4</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
+      <c r="E226">
+        <v>2</v>
+      </c>
+      <c r="F226">
+        <v>1</v>
+      </c>
+      <c r="G226">
+        <v>1</v>
+      </c>
+      <c r="H226">
+        <v>4</v>
+      </c>
+      <c r="I226">
+        <v>2</v>
+      </c>
+      <c r="J226">
+        <v>2</v>
+      </c>
+      <c r="K226">
+        <v>1</v>
+      </c>
+      <c r="L226">
+        <v>2</v>
+      </c>
+      <c r="M226">
+        <v>6</v>
+      </c>
+      <c r="N226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>22</v>
+      </c>
+      <c r="B227" t="s">
+        <v>23</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+      <c r="D227">
+        <v>2</v>
+      </c>
+      <c r="E227">
+        <v>2</v>
+      </c>
+      <c r="F227">
+        <v>1</v>
+      </c>
+      <c r="G227">
+        <v>1</v>
+      </c>
+      <c r="H227">
+        <v>4</v>
+      </c>
+      <c r="I227">
+        <v>2</v>
+      </c>
+      <c r="J227">
+        <v>2</v>
+      </c>
+      <c r="K227">
+        <v>1</v>
+      </c>
+      <c r="L227">
+        <v>2</v>
+      </c>
+      <c r="M227">
+        <v>3</v>
+      </c>
+      <c r="N227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>22</v>
+      </c>
+      <c r="B228" t="s">
+        <v>23</v>
+      </c>
+      <c r="C228">
+        <v>5</v>
+      </c>
+      <c r="D228">
+        <v>3</v>
+      </c>
+      <c r="E228">
+        <v>1</v>
+      </c>
+      <c r="F228">
+        <v>2</v>
+      </c>
+      <c r="G228">
+        <v>2</v>
+      </c>
+      <c r="H228">
+        <v>4</v>
+      </c>
+      <c r="I228">
+        <v>2</v>
+      </c>
+      <c r="J228">
+        <v>2</v>
+      </c>
+      <c r="K228">
+        <v>1</v>
+      </c>
+      <c r="L228">
+        <v>1</v>
+      </c>
+      <c r="M228">
+        <v>3</v>
+      </c>
+      <c r="N228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>22</v>
+      </c>
+      <c r="B229" t="s">
+        <v>23</v>
+      </c>
+      <c r="C229">
+        <v>5</v>
+      </c>
+      <c r="D229">
+        <v>3</v>
+      </c>
+      <c r="E229">
+        <v>3</v>
+      </c>
+      <c r="F229">
+        <v>3</v>
+      </c>
+      <c r="G229">
+        <v>2</v>
+      </c>
+      <c r="H229">
+        <v>6</v>
+      </c>
+      <c r="I229">
+        <v>5</v>
+      </c>
+      <c r="J229">
+        <v>2</v>
+      </c>
+      <c r="K229">
+        <v>2</v>
+      </c>
+      <c r="L229">
+        <v>3</v>
+      </c>
+      <c r="M229">
+        <v>4</v>
+      </c>
+      <c r="N229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>22</v>
+      </c>
+      <c r="B230" t="s">
+        <v>23</v>
+      </c>
+      <c r="C230">
+        <v>5</v>
+      </c>
+      <c r="D230">
+        <v>3</v>
+      </c>
+      <c r="E230">
+        <v>3</v>
+      </c>
+      <c r="F230">
+        <v>3</v>
+      </c>
+      <c r="G230">
+        <v>3</v>
+      </c>
+      <c r="H230">
+        <v>6</v>
+      </c>
+      <c r="I230">
+        <v>5</v>
+      </c>
+      <c r="J230">
+        <v>3</v>
+      </c>
+      <c r="K230">
+        <v>2</v>
+      </c>
+      <c r="L230">
+        <v>3</v>
+      </c>
+      <c r="M230">
+        <v>6</v>
+      </c>
+      <c r="N230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>22</v>
+      </c>
+      <c r="B231" t="s">
+        <v>23</v>
+      </c>
+      <c r="C231">
+        <v>6</v>
+      </c>
+      <c r="D231">
+        <v>4</v>
+      </c>
+      <c r="E231">
+        <v>4</v>
+      </c>
+      <c r="F231">
+        <v>3</v>
+      </c>
+      <c r="G231">
+        <v>5</v>
+      </c>
+      <c r="H231">
+        <v>6</v>
+      </c>
+      <c r="I231">
+        <v>0</v>
+      </c>
+      <c r="J231">
+        <v>5</v>
+      </c>
+      <c r="K231">
+        <v>3</v>
+      </c>
+      <c r="L231">
+        <v>4</v>
+      </c>
+      <c r="M231">
+        <v>6</v>
+      </c>
+      <c r="N231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>22</v>
+      </c>
+      <c r="B232" t="s">
+        <v>23</v>
+      </c>
+      <c r="C232">
+        <v>6</v>
+      </c>
+      <c r="D232">
+        <v>4</v>
+      </c>
+      <c r="E232">
+        <v>5</v>
+      </c>
+      <c r="F232">
+        <v>2</v>
+      </c>
+      <c r="G232">
+        <v>2</v>
+      </c>
+      <c r="H232">
+        <v>6</v>
+      </c>
+      <c r="I232">
+        <v>0</v>
+      </c>
+      <c r="J232">
+        <v>3</v>
+      </c>
+      <c r="K232">
+        <v>3</v>
+      </c>
+      <c r="L232">
+        <v>5</v>
+      </c>
+      <c r="M232">
+        <v>6</v>
+      </c>
+      <c r="N232">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>22</v>
+      </c>
+      <c r="B233" t="s">
+        <v>23</v>
+      </c>
+      <c r="C233">
+        <v>0</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>0</v>
+      </c>
+      <c r="F233">
+        <v>0</v>
+      </c>
+      <c r="G233">
+        <v>0</v>
+      </c>
+      <c r="H233">
+        <v>0</v>
+      </c>
+      <c r="I233">
+        <v>0</v>
+      </c>
+      <c r="J233">
+        <v>0</v>
+      </c>
+      <c r="K233">
+        <v>0</v>
+      </c>
+      <c r="L233">
+        <v>0</v>
+      </c>
+      <c r="M233">
+        <v>0</v>
+      </c>
+      <c r="N233">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>22</v>
+      </c>
+      <c r="B234" t="s">
+        <v>23</v>
+      </c>
+      <c r="C234">
+        <v>0</v>
+      </c>
+      <c r="D234">
+        <v>0</v>
+      </c>
+      <c r="E234">
+        <v>0</v>
+      </c>
+      <c r="F234">
+        <v>5</v>
+      </c>
+      <c r="G234">
+        <v>0</v>
+      </c>
+      <c r="H234">
+        <v>0</v>
+      </c>
+      <c r="I234">
+        <v>0</v>
+      </c>
+      <c r="J234">
+        <v>0</v>
+      </c>
+      <c r="K234">
+        <v>0</v>
+      </c>
+      <c r="L234">
+        <v>0</v>
+      </c>
+      <c r="M234">
+        <v>0</v>
+      </c>
+      <c r="N234">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>22</v>
+      </c>
+      <c r="B235" t="s">
+        <v>23</v>
+      </c>
+      <c r="C235">
+        <v>6</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>0</v>
+      </c>
+      <c r="F235">
+        <v>0</v>
+      </c>
+      <c r="G235">
+        <v>0</v>
+      </c>
+      <c r="H235">
+        <v>0</v>
+      </c>
+      <c r="I235">
+        <v>0</v>
+      </c>
+      <c r="J235">
+        <v>0</v>
+      </c>
+      <c r="K235">
+        <v>0</v>
+      </c>
+      <c r="L235">
+        <v>0</v>
+      </c>
+      <c r="M235">
+        <v>0</v>
+      </c>
+      <c r="N235">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>22</v>
+      </c>
+      <c r="B236" t="s">
+        <v>23</v>
+      </c>
+      <c r="C236">
+        <v>0</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>0</v>
+      </c>
+      <c r="F236">
+        <v>0</v>
+      </c>
+      <c r="G236">
+        <v>0</v>
+      </c>
+      <c r="H236">
+        <v>0</v>
+      </c>
+      <c r="I236">
+        <v>0</v>
+      </c>
+      <c r="J236">
+        <v>0</v>
+      </c>
+      <c r="K236">
+        <v>0</v>
+      </c>
+      <c r="L236">
+        <v>0</v>
+      </c>
+      <c r="M236">
+        <v>0</v>
+      </c>
+      <c r="N236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>22</v>
+      </c>
+      <c r="B237" t="s">
+        <v>23</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+      <c r="E237">
+        <v>0</v>
+      </c>
+      <c r="F237">
+        <v>0</v>
+      </c>
+      <c r="G237">
+        <v>0</v>
+      </c>
+      <c r="H237">
+        <v>0</v>
+      </c>
+      <c r="I237">
+        <v>0</v>
+      </c>
+      <c r="J237">
+        <v>0</v>
+      </c>
+      <c r="K237">
+        <v>0</v>
+      </c>
+      <c r="L237">
+        <v>0</v>
+      </c>
+      <c r="M237">
+        <v>0</v>
+      </c>
+      <c r="N237">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>